<commit_message>
commit before migrating to 206
</commit_message>
<xml_diff>
--- a/app/config/tables/distribution/forms/distribution/distribution.xlsx
+++ b/app/config/tables/distribution/forms/distribution/distribution.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>type</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>model.isSessionVariable</t>
+  </si>
+  <si>
+    <t>is_override</t>
   </si>
 </sst>
 </file>
@@ -1142,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -1241,6 +1244,14 @@
       </c>
       <c r="B11" s="5" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>